<commit_message>
Update: Added logging functionalities, Data Verification, Determine Results
Signed-off-by: Kway Yi Shen <kwayyishen@gmail.com>
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>team1</t>
+          <t>Team1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -524,116 +524,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16/03</t>
+          <t>15/12</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>team3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>16/03</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>team4</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>16/03</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>7</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>team5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>03/12</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
         <v>2</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>